<commit_message>
add claude 3.5 haiku and sonnet
</commit_message>
<xml_diff>
--- a/excels/MHPP_ICLR.xlsx
+++ b/excels/MHPP_ICLR.xlsx
@@ -13,17 +13,17 @@
     <sheet state="visible" name="mhpp-he-correlation" sheetId="8" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_1651915F_2B76_47EA_B69D_2794E1F56E41_.wvu.FilterData">'MHPP Problem Set'!$J$1:$J$1071</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_91B5F322_97C1_4F70_B73C_AB71AFFDC418_.wvu.FilterData">'MHPP Problem Set'!$J$1:$J$1071</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{1651915F-2B76-47EA-B69D-2794E1F56E41}" name="过滤器1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{91B5F322-97C1-4F70-B73C-AB71AFFDC418}" name="过滤器1"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2033" uniqueCount="1096">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2069" uniqueCount="1100">
   <si>
     <t>array泛滥，所以对于多于4个topic的情况，删去其中含有的array</t>
   </si>
@@ -3579,7 +3579,7 @@
     <t>Greedy distraction</t>
   </si>
   <si>
-    <t>Greedy redefinition</t>
+    <t>Greedy redefination</t>
   </si>
   <si>
     <t>Greedy shortcut</t>
@@ -3600,46 +3600,49 @@
     <t>Distraction pass@1</t>
   </si>
   <si>
-    <t>Distraction  pass@5</t>
-  </si>
-  <si>
-    <t>Redefinition  pass@1</t>
-  </si>
-  <si>
-    <t>Redefinition  pass@5</t>
-  </si>
-  <si>
-    <t>Shortcut  pass@1</t>
-  </si>
-  <si>
-    <t>Shortcut  pass@5</t>
-  </si>
-  <si>
-    <t>Commonsense  pass@1</t>
-  </si>
-  <si>
-    <t>Commonsense  pass@5</t>
-  </si>
-  <si>
-    <t>Cornercase  pass@1</t>
-  </si>
-  <si>
-    <t>Complex  pass@1</t>
-  </si>
-  <si>
-    <t>Complex  pass@5</t>
-  </si>
-  <si>
-    <t>Codesense  pass@1</t>
-  </si>
-  <si>
-    <t>Codesense  pass@5</t>
+    <t>Distraction pass@5</t>
+  </si>
+  <si>
+    <t>Redefinition pass@1</t>
+  </si>
+  <si>
+    <t>Redefinition pass@5</t>
+  </si>
+  <si>
+    <t>Shortcut pass@1</t>
+  </si>
+  <si>
+    <t>Shortcut pass@5</t>
+  </si>
+  <si>
+    <t>Commonsense pass@1</t>
+  </si>
+  <si>
+    <t>Commonsense pass@5</t>
+  </si>
+  <si>
+    <t>Cornercase pass@1</t>
+  </si>
+  <si>
+    <t>Cornercase pass@5</t>
+  </si>
+  <si>
+    <t>Complex pass@1</t>
+  </si>
+  <si>
+    <t>Complex pass@5</t>
+  </si>
+  <si>
+    <t>Codesense pass@1</t>
+  </si>
+  <si>
+    <t>Codesense pass@5</t>
   </si>
   <si>
     <t>pass@1</t>
   </si>
   <si>
-    <t xml:space="preserve"> pass@5</t>
+    <t>pass@5</t>
   </si>
   <si>
     <t>GPT-4o-2024-05-13</t>
@@ -3778,6 +3781,15 @@
   </si>
   <si>
     <t>Gemma2 IT 27B</t>
+  </si>
+  <si>
+    <t>Claude 3.5 Sonnet 20241022</t>
+  </si>
+  <si>
+    <t>Claude 3 Haiku 20241022</t>
+  </si>
+  <si>
+    <t>https://www.anthropic.com/claude/haiku</t>
   </si>
   <si>
     <t>postprocess merged</t>
@@ -4552,11 +4564,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1020616290"/>
-        <c:axId val="500592808"/>
+        <c:axId val="1864167271"/>
+        <c:axId val="1851316506"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1020616290"/>
+        <c:axId val="1864167271"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4608,10 +4620,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="500592808"/>
+        <c:crossAx val="1851316506"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="500592808"/>
+        <c:axId val="1851316506"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4686,7 +4698,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1020616290"/>
+        <c:crossAx val="1864167271"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -9985,7 +9997,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{1651915F-2B76-47EA-B69D-2794E1F56E41}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{91B5F322-97C1-4F70-B73C-AB71AFFDC418}" filter="1" showAutoFilter="1">
       <autoFilter ref="$J$1:$J$1071"/>
     </customSheetView>
   </customSheetViews>
@@ -12023,33 +12035,33 @@
         <v>982</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="C2" s="1" t="b">
         <v>1</v>
@@ -12129,10 +12141,10 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="C3" s="1" t="b">
         <v>1</v>
@@ -12212,10 +12224,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C4" s="1" t="b">
         <v>1</v>
@@ -12295,10 +12307,10 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="C5" s="1" t="b">
         <v>1</v>
@@ -12378,10 +12390,10 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="C6" s="1" t="b">
         <v>1</v>
@@ -12461,10 +12473,10 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="C7" s="1" t="b">
         <v>1</v>
@@ -12544,10 +12556,10 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="C8" s="1" t="b">
         <v>1</v>
@@ -12627,10 +12639,10 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="C9" s="1" t="b">
         <v>1</v>
@@ -12710,10 +12722,10 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="C10" s="1" t="b">
         <v>1</v>
@@ -12793,10 +12805,10 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>1007</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C11" s="1" t="b">
         <v>1</v>
@@ -12879,7 +12891,7 @@
         <v>960</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="C12" s="1" t="b">
         <v>1</v>
@@ -12959,10 +12971,10 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="C13" s="1" t="b">
         <v>1</v>
@@ -13042,10 +13054,10 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="C14" s="1" t="b">
         <v>1</v>
@@ -13125,10 +13137,10 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="C15" s="1" t="b">
         <v>1</v>
@@ -13211,7 +13223,7 @@
         <v>945</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="C16" s="1" t="b">
         <v>1</v>
@@ -13294,7 +13306,7 @@
         <v>946</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C17" s="1" t="b">
         <v>1</v>
@@ -13377,7 +13389,7 @@
         <v>947</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="C18" s="1" t="b">
         <v>1</v>
@@ -13457,10 +13469,10 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="C19" s="1" t="b">
         <v>1</v>
@@ -13490,60 +13502,60 @@
         <v>68.1</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="X19" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Z19" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="AA19" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="C20" s="1" t="b">
         <v>1</v>
@@ -13573,60 +13585,60 @@
         <v>66.2</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="X20" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Z20" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="AA20" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="C21" s="1" t="b">
         <v>1</v>
@@ -13656,60 +13668,60 @@
         <v>45.2</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="V21" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="W21" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="X21" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Y21" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Z21" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="AA21" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="C22" s="1" t="b">
         <v>1</v>
@@ -13739,60 +13751,60 @@
         <v>24.8</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="X22" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Z22" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="AA22" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="C23" s="1" t="b">
         <v>1</v>
@@ -13822,52 +13834,52 @@
         <v>39.5</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="X23" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Y23" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Z23" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="AA23" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="24">
@@ -13875,7 +13887,7 @@
         <v>949</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="C24" s="1" t="b">
         <v>1</v>
@@ -13905,52 +13917,52 @@
         <v>33.8</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="V24" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="X24" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Y24" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Z24" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="AA24" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="25">
@@ -13958,7 +13970,7 @@
         <v>955</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C25" s="1" t="b">
         <v>1</v>
@@ -13988,60 +14000,60 @@
         <v>41.4</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="T25" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="V25" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="X25" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Y25" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Z25" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="AA25" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="C26" s="1" t="b">
         <v>1</v>
@@ -14071,60 +14083,60 @@
         <v>20.0</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="T26" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="X26" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Y26" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Z26" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="AA26" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="C27" s="1" t="b">
         <v>1</v>
@@ -14154,52 +14166,52 @@
         <v>21.9</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="T27" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="U27" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="V27" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="W27" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="X27" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Y27" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Z27" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="AA27" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="28">
@@ -14207,7 +14219,7 @@
         <v>963</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="C28" s="1" t="b">
         <v>1</v>
@@ -14237,60 +14249,60 @@
         <v>11.0</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="T28" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="V28" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="W28" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="X28" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Y28" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Z28" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="AA28" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="C29" s="1" t="b">
         <v>1</v>
@@ -14320,52 +14332,218 @@
         <v>28.6</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="S29" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="T29" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="U29" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="V29" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="W29" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="X29" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Y29" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="Z29" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="AA29" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C30" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>33.3</v>
+      </c>
+      <c r="G30" s="1">
+        <v>46.7</v>
+      </c>
+      <c r="H30" s="1">
+        <v>40.0</v>
+      </c>
+      <c r="I30" s="1">
+        <v>43.3</v>
+      </c>
+      <c r="J30" s="1">
+        <v>53.3</v>
+      </c>
+      <c r="K30" s="1">
+        <v>48.1</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="T30" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="U30" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="V30" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="W30" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="X30" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="Y30" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="Z30" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="AA30" s="1" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C31" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>43.3</v>
+      </c>
+      <c r="E31" s="1">
+        <v>43.3</v>
+      </c>
+      <c r="F31" s="1">
+        <v>36.7</v>
+      </c>
+      <c r="G31" s="1">
+        <v>40.0</v>
+      </c>
+      <c r="H31" s="1">
+        <v>40.0</v>
+      </c>
+      <c r="I31" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="J31" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="K31" s="1">
+        <v>40.5</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="U31" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="V31" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="W31" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="X31" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="Y31" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="Z31" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="AA31" s="1" t="s">
+        <v>1021</v>
       </c>
     </row>
   </sheetData>
@@ -14398,8 +14576,10 @@
     <hyperlink r:id="rId26" ref="B27"/>
     <hyperlink r:id="rId27" ref="B28"/>
     <hyperlink r:id="rId28" ref="B29"/>
+    <hyperlink r:id="rId29" ref="B30"/>
+    <hyperlink r:id="rId30" ref="B31"/>
   </hyperlinks>
-  <drawing r:id="rId29"/>
+  <drawing r:id="rId31"/>
 </worksheet>
 </file>
 
@@ -14430,7 +14610,7 @@
         <v>230</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1035</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="2">
@@ -14448,31 +14628,31 @@
     </row>
     <row r="3">
       <c r="C3" s="39" t="s">
-        <v>1036</v>
+        <v>1040</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1037</v>
+        <v>1041</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>1038</v>
+        <v>1042</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>1039</v>
+        <v>1043</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>1040</v>
+        <v>1044</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1041</v>
+        <v>1045</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>1042</v>
+        <v>1046</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>1043</v>
+        <v>1047</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>1044</v>
+        <v>1048</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>636</v>
@@ -14482,7 +14662,7 @@
     <row r="4">
       <c r="C4" s="38"/>
       <c r="D4" s="8" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="E4" s="33">
         <v>0.5</v>
@@ -14513,7 +14693,7 @@
     <row r="5">
       <c r="C5" s="38"/>
       <c r="D5" s="8" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="E5" s="33">
         <v>0.36667</v>
@@ -14544,7 +14724,7 @@
     <row r="6">
       <c r="C6" s="38"/>
       <c r="D6" s="8" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="E6" s="33">
         <v>0.43333</v>
@@ -14575,7 +14755,7 @@
     <row r="7">
       <c r="C7" s="38"/>
       <c r="D7" s="8" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="E7" s="33">
         <v>0.46667</v>
@@ -14637,7 +14817,7 @@
     <row r="9">
       <c r="C9" s="38"/>
       <c r="D9" s="1" t="s">
-        <v>1045</v>
+        <v>1049</v>
       </c>
       <c r="E9" s="33">
         <v>0.33333</v>
@@ -14696,7 +14876,7 @@
       </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="8" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="R10" s="33">
         <v>0.36667</v>
@@ -14754,7 +14934,7 @@
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="R11" s="33">
         <v>0.3</v>
@@ -14815,7 +14995,7 @@
     <row r="13">
       <c r="C13" s="38"/>
       <c r="D13" s="8" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E13" s="33">
         <v>0.3</v>
@@ -14846,7 +15026,7 @@
     <row r="14">
       <c r="C14" s="38"/>
       <c r="D14" s="1" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="E14" s="33">
         <v>0.26667</v>
@@ -14877,7 +15057,7 @@
     <row r="15">
       <c r="C15" s="38"/>
       <c r="D15" s="1" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="E15" s="33">
         <v>0.3</v>
@@ -14939,7 +15119,7 @@
     <row r="17">
       <c r="C17" s="38"/>
       <c r="D17" s="1" t="s">
-        <v>1046</v>
+        <v>1050</v>
       </c>
       <c r="E17" s="33">
         <v>0.13333</v>
@@ -15001,7 +15181,7 @@
     <row r="19">
       <c r="C19" s="38"/>
       <c r="D19" s="1" t="s">
-        <v>1047</v>
+        <v>1051</v>
       </c>
       <c r="E19" s="33">
         <v>0.2</v>
@@ -15032,7 +15212,7 @@
     <row r="20">
       <c r="C20" s="38"/>
       <c r="D20" s="1" t="s">
-        <v>1048</v>
+        <v>1052</v>
       </c>
       <c r="E20" s="33">
         <v>0.16667</v>
@@ -15063,7 +15243,7 @@
     <row r="21">
       <c r="C21" s="38"/>
       <c r="D21" s="1" t="s">
-        <v>1049</v>
+        <v>1053</v>
       </c>
       <c r="E21" s="33">
         <v>0.2</v>
@@ -15094,7 +15274,7 @@
     <row r="22">
       <c r="C22" s="38"/>
       <c r="D22" s="1" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="E22" s="33">
         <v>0.2</v>
@@ -15187,7 +15367,7 @@
     <row r="25">
       <c r="C25" s="38"/>
       <c r="D25" s="1" t="s">
-        <v>1050</v>
+        <v>1054</v>
       </c>
       <c r="E25" s="33">
         <v>0.1</v>
@@ -15218,7 +15398,7 @@
     <row r="26">
       <c r="C26" s="38"/>
       <c r="D26" s="1" t="s">
-        <v>1051</v>
+        <v>1055</v>
       </c>
       <c r="E26" s="33">
         <v>0.06667</v>
@@ -15248,10 +15428,10 @@
     </row>
     <row r="27">
       <c r="C27" s="39" t="s">
-        <v>1052</v>
+        <v>1056</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="E27" s="40">
         <v>0.8</v>
@@ -15282,7 +15462,7 @@
     <row r="28">
       <c r="C28" s="38"/>
       <c r="D28" s="1" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="E28" s="40">
         <v>0.7</v>
@@ -15468,7 +15648,7 @@
     <row r="37">
       <c r="C37" s="38"/>
       <c r="D37" s="1" t="s">
-        <v>1053</v>
+        <v>1057</v>
       </c>
       <c r="E37" s="39"/>
       <c r="F37" s="39"/>
@@ -15479,60 +15659,60 @@
       <c r="K37" s="39"/>
       <c r="L37" s="39"/>
       <c r="P37" s="1" t="s">
-        <v>1054</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="38">
       <c r="D38" s="1" t="s">
-        <v>1037</v>
+        <v>1041</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>1038</v>
+        <v>1042</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>1039</v>
+        <v>1043</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>1040</v>
+        <v>1044</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>1041</v>
+        <v>1045</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>1042</v>
+        <v>1046</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>1043</v>
+        <v>1047</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>1044</v>
+        <v>1048</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>636</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>1037</v>
+        <v>1041</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>1038</v>
+        <v>1042</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>1039</v>
+        <v>1043</v>
       </c>
       <c r="S38" s="1" t="s">
-        <v>1040</v>
+        <v>1044</v>
       </c>
       <c r="T38" s="1" t="s">
-        <v>1041</v>
+        <v>1045</v>
       </c>
       <c r="U38" s="1" t="s">
-        <v>1042</v>
+        <v>1046</v>
       </c>
       <c r="V38" s="1" t="s">
-        <v>1043</v>
+        <v>1047</v>
       </c>
       <c r="W38" s="1" t="s">
-        <v>1044</v>
+        <v>1048</v>
       </c>
       <c r="X38" s="1" t="s">
         <v>636</v>
@@ -15540,7 +15720,7 @@
     </row>
     <row r="39">
       <c r="D39" s="1" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="E39" s="33">
         <v>0.5</v>
@@ -15567,7 +15747,7 @@
         <v>0.481</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="Q39" s="33">
         <v>0.4667</v>
@@ -15596,7 +15776,7 @@
     </row>
     <row r="40">
       <c r="D40" s="1" t="s">
-        <v>1055</v>
+        <v>1059</v>
       </c>
       <c r="E40" s="33">
         <v>0.3333</v>
@@ -15623,7 +15803,7 @@
         <v>0.4476</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>1055</v>
+        <v>1059</v>
       </c>
       <c r="Q40" s="33"/>
       <c r="R40" s="33"/>
@@ -15636,7 +15816,7 @@
     </row>
     <row r="41">
       <c r="D41" s="1" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="E41" s="33">
         <v>0.4333</v>
@@ -15663,7 +15843,7 @@
         <v>0.4286</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="Q41" s="33"/>
       <c r="R41" s="33"/>
@@ -15716,7 +15896,7 @@
     </row>
     <row r="43">
       <c r="D43" s="1" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="E43" s="33">
         <v>0.4667</v>
@@ -15743,7 +15923,7 @@
         <v>0.3952</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="Q43" s="33"/>
       <c r="R43" s="33"/>
@@ -15756,7 +15936,7 @@
     </row>
     <row r="44">
       <c r="D44" s="1" t="s">
-        <v>1045</v>
+        <v>1049</v>
       </c>
       <c r="E44" s="33">
         <v>0.3333</v>
@@ -15783,7 +15963,7 @@
         <v>0.3905</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>1045</v>
+        <v>1049</v>
       </c>
       <c r="Q44" s="33"/>
       <c r="R44" s="33"/>
@@ -15916,7 +16096,7 @@
     </row>
     <row r="48">
       <c r="D48" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E48" s="33">
         <v>0.3</v>
@@ -15943,7 +16123,7 @@
         <v>0.2667</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="Q48" s="33"/>
       <c r="R48" s="33"/>
@@ -15956,7 +16136,7 @@
     </row>
     <row r="49">
       <c r="D49" s="1" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="E49" s="33">
         <v>0.2667</v>
@@ -15983,7 +16163,7 @@
         <v>0.2476</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="Q49" s="33"/>
       <c r="R49" s="33"/>
@@ -15996,7 +16176,7 @@
     </row>
     <row r="50">
       <c r="D50" s="1" t="s">
-        <v>1056</v>
+        <v>1060</v>
       </c>
       <c r="E50" s="33">
         <v>0.3</v>
@@ -16023,7 +16203,7 @@
         <v>0.2429</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>1056</v>
+        <v>1060</v>
       </c>
       <c r="Q50" s="33"/>
       <c r="R50" s="33"/>
@@ -16116,7 +16296,7 @@
     </row>
     <row r="53">
       <c r="D53" s="1" t="s">
-        <v>1046</v>
+        <v>1050</v>
       </c>
       <c r="E53" s="33">
         <v>0.1333</v>
@@ -16143,7 +16323,7 @@
         <v>0.2</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>1046</v>
+        <v>1050</v>
       </c>
       <c r="Q53" s="33"/>
       <c r="R53" s="33"/>
@@ -16156,7 +16336,7 @@
     </row>
     <row r="54">
       <c r="D54" s="1" t="s">
-        <v>1047</v>
+        <v>1051</v>
       </c>
       <c r="E54" s="33">
         <v>0.2</v>
@@ -16183,7 +16363,7 @@
         <v>0.1905</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>1047</v>
+        <v>1051</v>
       </c>
       <c r="Q54" s="33"/>
       <c r="R54" s="33"/>
@@ -16196,7 +16376,7 @@
     </row>
     <row r="55">
       <c r="D55" s="1" t="s">
-        <v>1048</v>
+        <v>1052</v>
       </c>
       <c r="E55" s="33">
         <v>0.1667</v>
@@ -16223,7 +16403,7 @@
         <v>0.1857</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>1048</v>
+        <v>1052</v>
       </c>
       <c r="Q55" s="33"/>
       <c r="R55" s="33"/>
@@ -16236,7 +16416,7 @@
     </row>
     <row r="56">
       <c r="D56" s="1" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="E56" s="33">
         <v>0.2</v>
@@ -16263,7 +16443,7 @@
         <v>0.1714</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="Q56" s="33"/>
       <c r="R56" s="33"/>
@@ -16276,7 +16456,7 @@
     </row>
     <row r="57">
       <c r="D57" s="1" t="s">
-        <v>1049</v>
+        <v>1053</v>
       </c>
       <c r="E57" s="33">
         <v>0.2</v>
@@ -16303,7 +16483,7 @@
         <v>0.1714</v>
       </c>
       <c r="P57" s="1" t="s">
-        <v>1049</v>
+        <v>1053</v>
       </c>
       <c r="Q57" s="33"/>
       <c r="R57" s="33"/>
@@ -16396,7 +16576,7 @@
     </row>
     <row r="60">
       <c r="D60" s="1" t="s">
-        <v>1050</v>
+        <v>1054</v>
       </c>
       <c r="E60" s="33">
         <v>0.1</v>
@@ -16423,7 +16603,7 @@
         <v>0.0857</v>
       </c>
       <c r="P60" s="1" t="s">
-        <v>1050</v>
+        <v>1054</v>
       </c>
       <c r="Q60" s="33"/>
       <c r="R60" s="33"/>
@@ -16436,7 +16616,7 @@
     </row>
     <row r="61">
       <c r="D61" s="1" t="s">
-        <v>1051</v>
+        <v>1055</v>
       </c>
       <c r="E61" s="33">
         <v>0.0667</v>
@@ -16463,7 +16643,7 @@
         <v>0.0762</v>
       </c>
       <c r="P61" s="1" t="s">
-        <v>1051</v>
+        <v>1055</v>
       </c>
       <c r="Q61" s="33"/>
       <c r="R61" s="33"/>
@@ -16479,28 +16659,28 @@
     </row>
     <row r="139">
       <c r="D139" s="1" t="s">
-        <v>1057</v>
+        <v>1061</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>1038</v>
+        <v>1042</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>1039</v>
+        <v>1043</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>1040</v>
+        <v>1044</v>
       </c>
       <c r="H139" s="1" t="s">
-        <v>1041</v>
+        <v>1045</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>1042</v>
+        <v>1046</v>
       </c>
       <c r="J139" s="1" t="s">
-        <v>1043</v>
+        <v>1047</v>
       </c>
       <c r="K139" s="1" t="s">
-        <v>1044</v>
+        <v>1048</v>
       </c>
       <c r="L139" s="1" t="s">
         <v>636</v>
@@ -16508,7 +16688,7 @@
     </row>
     <row r="140">
       <c r="D140" s="1" t="s">
-        <v>1058</v>
+        <v>1062</v>
       </c>
       <c r="E140" s="33">
         <v>0.4</v>
@@ -16537,7 +16717,7 @@
     </row>
     <row r="141">
       <c r="D141" s="1" t="s">
-        <v>1059</v>
+        <v>1063</v>
       </c>
       <c r="E141" s="33">
         <v>0.4</v>
@@ -16566,7 +16746,7 @@
     </row>
     <row r="142">
       <c r="D142" s="1" t="s">
-        <v>1060</v>
+        <v>1064</v>
       </c>
       <c r="E142" s="33">
         <v>0.4</v>
@@ -16595,7 +16775,7 @@
     </row>
     <row r="143">
       <c r="D143" s="1" t="s">
-        <v>1061</v>
+        <v>1065</v>
       </c>
       <c r="E143" s="33">
         <v>0.4</v>
@@ -16644,7 +16824,7 @@
   <sheetData>
     <row r="3">
       <c r="B3" s="1" t="s">
-        <v>1062</v>
+        <v>1066</v>
       </c>
       <c r="D3" s="35" t="s">
         <v>951</v>
@@ -16674,7 +16854,7 @@
     <row r="4">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>1063</v>
+        <v>1067</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>953</v>
@@ -16728,10 +16908,10 @@
     <row r="5">
       <c r="A5" s="1"/>
       <c r="B5" s="8" t="s">
-        <v>1064</v>
+        <v>1068</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="D5" s="1">
         <v>52.9</v>
@@ -16785,10 +16965,10 @@
     <row r="6">
       <c r="A6" s="1"/>
       <c r="B6" s="8" t="s">
-        <v>1064</v>
+        <v>1068</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="D6" s="1">
         <v>44.4</v>
@@ -16842,10 +17022,10 @@
     <row r="7">
       <c r="A7" s="1"/>
       <c r="B7" s="8" t="s">
-        <v>1064</v>
+        <v>1068</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="D7" s="1">
         <v>42.5</v>
@@ -16899,10 +17079,10 @@
     <row r="8">
       <c r="A8" s="1"/>
       <c r="B8" s="8" t="s">
-        <v>1064</v>
+        <v>1068</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="D8" s="1">
         <v>29.6</v>
@@ -16955,10 +17135,10 @@
     </row>
     <row r="9">
       <c r="B9" s="8" t="s">
-        <v>1064</v>
+        <v>1068</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="D9" s="1">
         <v>37.8</v>
@@ -17012,10 +17192,10 @@
     <row r="10">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>1065</v>
+        <v>1069</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1066</v>
+        <v>1070</v>
       </c>
       <c r="D10" s="1">
         <v>16.8</v>
@@ -17068,10 +17248,10 @@
     </row>
     <row r="11">
       <c r="B11" s="1" t="s">
-        <v>1067</v>
+        <v>1071</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1068</v>
+        <v>1072</v>
       </c>
       <c r="D11" s="1">
         <v>15.4</v>
@@ -17125,10 +17305,10 @@
     <row r="12">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>1065</v>
+        <v>1069</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1069</v>
+        <v>1073</v>
       </c>
       <c r="D12" s="1">
         <v>12.5</v>
@@ -17181,10 +17361,10 @@
     </row>
     <row r="13">
       <c r="B13" s="1" t="s">
-        <v>1067</v>
+        <v>1071</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="D13" s="1">
         <v>6.8</v>
@@ -17238,18 +17418,18 @@
     <row r="14">
       <c r="A14" s="1"/>
       <c r="B14" s="21" t="s">
-        <v>1070</v>
+        <v>1074</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="1" t="s">
-        <v>1071</v>
+        <v>1075</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="D15" s="1">
         <v>15.7</v>
@@ -17302,10 +17482,10 @@
     </row>
     <row r="16">
       <c r="B16" s="1" t="s">
-        <v>1071</v>
+        <v>1075</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="D16" s="1">
         <v>8.6</v>
@@ -17358,10 +17538,10 @@
     </row>
     <row r="17">
       <c r="B17" s="1" t="s">
-        <v>1065</v>
+        <v>1069</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1072</v>
+        <v>1076</v>
       </c>
       <c r="D17" s="1">
         <v>6.7</v>
@@ -17415,10 +17595,10 @@
     <row r="18">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>1067</v>
+        <v>1071</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="D18" s="1">
         <v>28.9</v>
@@ -17472,7 +17652,7 @@
     <row r="19">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>1067</v>
+        <v>1071</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>945</v>
@@ -17529,7 +17709,7 @@
     <row r="20">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>1067</v>
+        <v>1071</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>946</v>
@@ -17586,7 +17766,7 @@
     <row r="21">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>1065</v>
+        <v>1069</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>947</v>
@@ -17642,7 +17822,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>1052</v>
+        <v>1056</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>960</v>
@@ -17698,17 +17878,17 @@
     </row>
     <row r="24">
       <c r="C24" s="42" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
     </row>
     <row r="25">
       <c r="C25" s="21" t="s">
-        <v>1055</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="26">
       <c r="C26" s="43" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
     </row>
     <row r="27">
@@ -17718,12 +17898,12 @@
     </row>
     <row r="28">
       <c r="C28" s="43" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
     </row>
     <row r="29">
       <c r="C29" s="43" t="s">
-        <v>1045</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="30">
@@ -17743,17 +17923,17 @@
     </row>
     <row r="33">
       <c r="C33" s="43" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
     </row>
     <row r="34">
       <c r="C34" s="43" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="35">
       <c r="C35" s="21" t="s">
-        <v>1056</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="36">
@@ -17768,27 +17948,27 @@
     </row>
     <row r="38">
       <c r="C38" s="43" t="s">
-        <v>1046</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="39">
       <c r="C39" s="43" t="s">
-        <v>1047</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="40">
       <c r="C40" s="43" t="s">
-        <v>1048</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="41">
       <c r="C41" s="43" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="42">
       <c r="C42" s="43" t="s">
-        <v>1049</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="43">
@@ -17803,32 +17983,32 @@
     </row>
     <row r="45">
       <c r="C45" s="42" t="s">
-        <v>1050</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="46">
       <c r="C46" s="42" t="s">
-        <v>1051</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="47">
       <c r="C47" s="42" t="s">
-        <v>1073</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="48">
       <c r="C48" s="42" t="s">
-        <v>1074</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="49">
       <c r="C49" s="42" t="s">
-        <v>1075</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" s="28" t="s">
-        <v>1076</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="53">
@@ -17859,7 +18039,7 @@
     </row>
     <row r="54">
       <c r="B54" s="1" t="s">
-        <v>1063</v>
+        <v>1067</v>
       </c>
       <c r="D54" s="17" t="s">
         <v>953</v>
@@ -17912,10 +18092,10 @@
     </row>
     <row r="55">
       <c r="B55" s="1" t="s">
-        <v>1064</v>
+        <v>1068</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="D55" s="1">
         <v>52.733</v>
@@ -17968,15 +18148,15 @@
     </row>
     <row r="56">
       <c r="C56" s="21" t="s">
-        <v>1055</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" s="1" t="s">
-        <v>1064</v>
+        <v>1068</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
     </row>
     <row r="58">
@@ -17986,10 +18166,10 @@
     </row>
     <row r="59">
       <c r="B59" s="1" t="s">
-        <v>1064</v>
+        <v>1068</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="D59" s="1">
         <v>44.533</v>
@@ -18042,10 +18222,10 @@
     </row>
     <row r="60">
       <c r="B60" s="1" t="s">
-        <v>1064</v>
+        <v>1068</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1045</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="61">
@@ -18060,7 +18240,7 @@
     </row>
     <row r="63">
       <c r="B63" s="1" t="s">
-        <v>1070</v>
+        <v>1074</v>
       </c>
       <c r="C63" s="43" t="s">
         <v>962</v>
@@ -18068,10 +18248,10 @@
     </row>
     <row r="64">
       <c r="B64" s="1" t="s">
-        <v>1064</v>
+        <v>1068</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="D64" s="1">
         <v>29.4</v>
@@ -18124,15 +18304,15 @@
     </row>
     <row r="65">
       <c r="B65" s="1" t="s">
-        <v>1065</v>
+        <v>1069</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="66">
       <c r="C66" s="21" t="s">
-        <v>1056</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="67">
@@ -18147,42 +18327,42 @@
     </row>
     <row r="69">
       <c r="B69" s="1" t="s">
-        <v>1065</v>
+        <v>1069</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1046</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="70">
       <c r="B70" s="1" t="s">
-        <v>1067</v>
+        <v>1071</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>1047</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="71">
       <c r="B71" s="1" t="s">
-        <v>1065</v>
+        <v>1069</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1048</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="72">
       <c r="B72" s="1" t="s">
-        <v>1067</v>
+        <v>1071</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="73">
       <c r="B73" s="1" t="s">
-        <v>1071</v>
+        <v>1075</v>
       </c>
       <c r="C73" s="43" t="s">
-        <v>1049</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="74">
@@ -18197,42 +18377,42 @@
     </row>
     <row r="76">
       <c r="B76" s="1" t="s">
-        <v>1071</v>
+        <v>1075</v>
       </c>
       <c r="C76" s="43" t="s">
-        <v>1050</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="77">
       <c r="B77" s="1" t="s">
-        <v>1067</v>
+        <v>1071</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>1051</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="78">
       <c r="B78" s="1" t="s">
-        <v>1067</v>
+        <v>1071</v>
       </c>
       <c r="C78" s="44" t="s">
-        <v>1073</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="79">
       <c r="B79" s="1" t="s">
-        <v>1067</v>
+        <v>1071</v>
       </c>
       <c r="C79" s="44" t="s">
-        <v>1074</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="80">
       <c r="B80" s="1" t="s">
-        <v>1065</v>
+        <v>1069</v>
       </c>
       <c r="C80" s="44" t="s">
-        <v>1075</v>
+        <v>1079</v>
       </c>
     </row>
   </sheetData>
@@ -18273,25 +18453,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>1077</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>1059</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>1058</v>
+        <v>1062</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1078</v>
+        <v>1082</v>
       </c>
       <c r="E4" s="45">
         <v>1.0</v>
@@ -18320,10 +18500,10 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>1079</v>
+        <v>1083</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="E5" s="46">
         <v>51.11</v>
@@ -18355,7 +18535,7 @@
         <v>945</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="E6" s="46">
         <v>42.07</v>
@@ -18384,10 +18564,10 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>1080</v>
+        <v>1084</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="E7" s="46">
         <v>45.19</v>
@@ -18416,7 +18596,7 @@
     </row>
     <row r="8">
       <c r="D8" s="1" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="E8" s="1">
         <v>44.27</v>
@@ -18532,7 +18712,7 @@
     </row>
     <row r="12">
       <c r="D12" s="14" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="E12" s="1">
         <v>15.96</v>
@@ -18561,7 +18741,7 @@
     </row>
     <row r="13">
       <c r="D13" s="1" t="s">
-        <v>1066</v>
+        <v>1070</v>
       </c>
       <c r="E13" s="23">
         <v>18.48</v>
@@ -18590,7 +18770,7 @@
     </row>
     <row r="14">
       <c r="D14" s="1" t="s">
-        <v>1081</v>
+        <v>1085</v>
       </c>
       <c r="E14" s="1">
         <v>15.05</v>
@@ -18619,7 +18799,7 @@
     </row>
     <row r="15">
       <c r="D15" s="1" t="s">
-        <v>1082</v>
+        <v>1086</v>
       </c>
       <c r="E15" s="1">
         <v>15.55</v>
@@ -18648,7 +18828,7 @@
     </row>
     <row r="19">
       <c r="D19" s="23" t="s">
-        <v>1083</v>
+        <v>1087</v>
       </c>
       <c r="E19" s="45">
         <v>1.0</v>
@@ -18677,7 +18857,7 @@
     </row>
     <row r="20">
       <c r="D20" s="1" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="E20" s="46">
         <v>0.09</v>
@@ -18706,7 +18886,7 @@
     </row>
     <row r="21">
       <c r="D21" s="1" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="E21" s="46">
         <v>0.1</v>
@@ -18735,7 +18915,7 @@
     </row>
     <row r="22">
       <c r="D22" s="1" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="E22" s="46">
         <v>0.14</v>
@@ -18764,7 +18944,7 @@
     </row>
     <row r="23">
       <c r="D23" s="1" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="E23" s="1">
         <v>0.1</v>
@@ -18880,7 +19060,7 @@
     </row>
     <row r="27">
       <c r="D27" s="14" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="E27" s="1">
         <v>0.1</v>
@@ -18909,7 +19089,7 @@
     </row>
     <row r="28">
       <c r="D28" s="1" t="s">
-        <v>1066</v>
+        <v>1070</v>
       </c>
       <c r="E28" s="1">
         <v>0.12</v>
@@ -18938,7 +19118,7 @@
     </row>
     <row r="29">
       <c r="D29" s="1" t="s">
-        <v>1081</v>
+        <v>1085</v>
       </c>
       <c r="E29" s="1">
         <v>0.18</v>
@@ -18967,7 +19147,7 @@
     </row>
     <row r="30">
       <c r="D30" s="1" t="s">
-        <v>1082</v>
+        <v>1086</v>
       </c>
       <c r="E30" s="1">
         <v>0.11</v>
@@ -19018,7 +19198,7 @@
     </row>
     <row r="34">
       <c r="D34" s="1" t="s">
-        <v>1084</v>
+        <v>1088</v>
       </c>
     </row>
   </sheetData>
@@ -19045,15 +19225,15 @@
     <row r="1">
       <c r="A1" s="47"/>
       <c r="B1" s="48" t="s">
-        <v>1085</v>
+        <v>1089</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>1086</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="48" t="s">
-        <v>1087</v>
+        <v>1091</v>
       </c>
       <c r="B2" s="49">
         <v>57.3</v>
@@ -19064,7 +19244,7 @@
     </row>
     <row r="3">
       <c r="A3" s="48" t="s">
-        <v>1088</v>
+        <v>1092</v>
       </c>
       <c r="B3" s="49">
         <v>61.0</v>
@@ -19075,7 +19255,7 @@
     </row>
     <row r="4">
       <c r="A4" s="48" t="s">
-        <v>1089</v>
+        <v>1093</v>
       </c>
       <c r="B4" s="49">
         <v>62.2</v>
@@ -19097,7 +19277,7 @@
     </row>
     <row r="6">
       <c r="A6" s="48" t="s">
-        <v>1090</v>
+        <v>1094</v>
       </c>
       <c r="B6" s="49">
         <v>72.0</v>
@@ -19119,7 +19299,7 @@
     </row>
     <row r="8">
       <c r="A8" s="48" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="B8" s="49">
         <v>72.6</v>
@@ -19141,7 +19321,7 @@
     </row>
     <row r="10">
       <c r="A10" s="48" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B10" s="49">
         <v>89.0</v>
@@ -19152,7 +19332,7 @@
     </row>
     <row r="11">
       <c r="A11" s="48" t="s">
-        <v>1091</v>
+        <v>1095</v>
       </c>
       <c r="B11" s="49">
         <v>87.2</v>
@@ -19163,7 +19343,7 @@
     </row>
     <row r="12">
       <c r="A12" s="48" t="s">
-        <v>1092</v>
+        <v>1096</v>
       </c>
       <c r="B12" s="49">
         <v>90.2</v>
@@ -19174,7 +19354,7 @@
     </row>
     <row r="13">
       <c r="A13" s="48" t="s">
-        <v>1093</v>
+        <v>1097</v>
       </c>
       <c r="B13" s="49">
         <v>81.7</v>
@@ -19185,7 +19365,7 @@
     </row>
     <row r="14">
       <c r="A14" s="48" t="s">
-        <v>1094</v>
+        <v>1098</v>
       </c>
       <c r="B14" s="49">
         <v>70.7</v>
@@ -19196,7 +19376,7 @@
     </row>
     <row r="15">
       <c r="A15" s="48" t="s">
-        <v>1050</v>
+        <v>1054</v>
       </c>
       <c r="B15" s="49">
         <v>17.7</v>
@@ -19218,7 +19398,7 @@
     </row>
     <row r="17">
       <c r="A17" s="48" t="s">
-        <v>1049</v>
+        <v>1053</v>
       </c>
       <c r="B17" s="49">
         <v>40.2</v>
@@ -19240,7 +19420,7 @@
     </row>
     <row r="19">
       <c r="A19" s="48" t="s">
-        <v>1045</v>
+        <v>1049</v>
       </c>
       <c r="B19" s="49">
         <v>89.0</v>
@@ -19251,7 +19431,7 @@
     </row>
     <row r="20">
       <c r="A20" s="48" t="s">
-        <v>1095</v>
+        <v>1099</v>
       </c>
       <c r="B20" s="49">
         <v>75.0</v>
@@ -19262,7 +19442,7 @@
     </row>
     <row r="21">
       <c r="A21" s="48" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="B21" s="49">
         <v>81.1</v>

</xml_diff>